<commit_message>
update state diagram as per robyn rename
</commit_message>
<xml_diff>
--- a/tests/state_diagram.xlsx
+++ b/tests/state_diagram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -42,7 +42,7 @@
     <t xml:space="preserve">-1 = must not be true</t>
   </si>
   <si>
-    <t xml:space="preserve">From ↓ to →</t>
+    <t xml:space="preserve">In ↓ you can be →</t>
   </si>
   <si>
     <t xml:space="preserve">susceptible</t>
@@ -332,7 +332,7 @@
   </sheetPr>
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -393,22 +393,22 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.43"/>
@@ -1181,16 +1181,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.43"/>

</xml_diff>

<commit_message>
rename vaccinations to doses
</commit_message>
<xml_diff>
--- a/tests/state_diagram.xlsx
+++ b/tests/state_diagram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -84,7 +84,7 @@
     <t xml:space="preserve">quarantined</t>
   </si>
   <si>
-    <t xml:space="preserve">vaccinations</t>
+    <t xml:space="preserve">vaccinated</t>
   </si>
 </sst>
 </file>
@@ -393,8 +393,8 @@
   </sheetPr>
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -461,7 +461,7 @@
         <v>quarantined</v>
       </c>
       <c r="O1" s="1" t="str">
-        <v>vaccinations</v>
+        <v>vaccinated</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1175,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1243,7 +1243,7 @@
         <v>quarantined</v>
       </c>
       <c r="O1" s="1" t="str">
-        <v>vaccinations</v>
+        <v>vaccinated</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>